<commit_message>
update pretrd for hait_ehfz
</commit_message>
<xml_diff>
--- a/data/input/trade_data_patch/huat/private_security_loan.xlsx
+++ b/data/input/trade_data_patch/huat/private_security_loan.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="596" uniqueCount="207">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="434" uniqueCount="164">
   <si>
     <t>证券代码</t>
   </si>
@@ -253,24 +253,15 @@
     <t>202101290000000776</t>
   </si>
   <si>
-    <t>600185</t>
-  </si>
-  <si>
-    <t>格力地产</t>
+    <t>601766</t>
+  </si>
+  <si>
+    <t>中国中车</t>
   </si>
   <si>
     <t>2021-01-28</t>
   </si>
   <si>
-    <t>202101280000001346</t>
-  </si>
-  <si>
-    <t>601766</t>
-  </si>
-  <si>
-    <t>中国中车</t>
-  </si>
-  <si>
     <t>202101280000001342</t>
   </si>
   <si>
@@ -457,15 +448,6 @@
     <t>202101250000001812</t>
   </si>
   <si>
-    <t>300123</t>
-  </si>
-  <si>
-    <t>亚光科技</t>
-  </si>
-  <si>
-    <t>202101250000001810</t>
-  </si>
-  <si>
     <t>2021-01-22</t>
   </si>
   <si>
@@ -493,78 +475,15 @@
     <t>202101210000000951</t>
   </si>
   <si>
-    <t>603005</t>
-  </si>
-  <si>
-    <t>晶方科技</t>
-  </si>
-  <si>
-    <t>202101210000000942</t>
-  </si>
-  <si>
-    <t>601058</t>
-  </si>
-  <si>
-    <t>赛轮轮胎</t>
-  </si>
-  <si>
-    <t>202101210000000939</t>
-  </si>
-  <si>
-    <t>600967</t>
-  </si>
-  <si>
-    <t>内蒙一机</t>
-  </si>
-  <si>
-    <t>202101210000000012</t>
-  </si>
-  <si>
-    <t>600893</t>
-  </si>
-  <si>
-    <t>航发动力</t>
-  </si>
-  <si>
-    <t>202101210000000011</t>
-  </si>
-  <si>
-    <t>600316</t>
-  </si>
-  <si>
-    <t>洪都航空</t>
-  </si>
-  <si>
-    <t>202101210000000010</t>
-  </si>
-  <si>
-    <t>600776</t>
-  </si>
-  <si>
-    <t>东方通信</t>
-  </si>
-  <si>
     <t>2021-01-20</t>
   </si>
   <si>
-    <t>202101200000001043</t>
-  </si>
-  <si>
-    <t>202101200000001035</t>
-  </si>
-  <si>
     <t>2021-02-16</t>
   </si>
   <si>
     <t>202101200000000956</t>
   </si>
   <si>
-    <t>202101200000000952</t>
-  </si>
-  <si>
-    <t>202101200000000048</t>
-  </si>
-  <si>
     <t>600460</t>
   </si>
   <si>
@@ -574,45 +493,6 @@
     <t>202101200000000047</t>
   </si>
   <si>
-    <t>300274</t>
-  </si>
-  <si>
-    <t>阳光电源</t>
-  </si>
-  <si>
-    <t>202101200000000046</t>
-  </si>
-  <si>
-    <t>2021-01-19</t>
-  </si>
-  <si>
-    <t>202101190000002143</t>
-  </si>
-  <si>
-    <t>600855</t>
-  </si>
-  <si>
-    <t>航天长峰</t>
-  </si>
-  <si>
-    <t>202101190000002142</t>
-  </si>
-  <si>
-    <t>202101190000002126</t>
-  </si>
-  <si>
-    <t>600197</t>
-  </si>
-  <si>
-    <t>伊力特</t>
-  </si>
-  <si>
-    <t>202101190000002124</t>
-  </si>
-  <si>
-    <t>202101190000002104</t>
-  </si>
-  <si>
     <t>2021-01-18</t>
   </si>
   <si>
@@ -626,23 +506,15 @@
   </si>
   <si>
     <t>202101180000000147</t>
-  </si>
-  <si>
-    <t>000733</t>
-  </si>
-  <si>
-    <t>振华科技</t>
-  </si>
-  <si>
-    <t>202101180000000145</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="176" formatCode="0.00 &quot;%&quot;"/>
+  <numFmts count="2">
+    <numFmt numFmtId="176" formatCode="0.000"/>
+    <numFmt numFmtId="177" formatCode="0.00 &quot;%&quot;"/>
   </numFmts>
   <fonts count="2">
     <font>
@@ -674,11 +546,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -974,7 +847,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:T65"/>
+  <dimension ref="A1:T47"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0"/>
   </sheetViews>
@@ -992,8 +865,8 @@
     <col min="10" max="10" width="30" style="2" customWidth="1"/>
     <col min="11" max="11" width="30" style="3" customWidth="1"/>
     <col min="12" max="12" width="30" style="3" customWidth="1"/>
-    <col min="13" max="13" width="30" style="2" customWidth="1"/>
-    <col min="14" max="14" width="30" style="2" customWidth="1"/>
+    <col min="13" max="13" width="30" style="4" customWidth="1"/>
+    <col min="14" max="14" width="30" style="4" customWidth="1"/>
     <col min="15" max="15" width="30" customWidth="1"/>
     <col min="16" max="16" width="30" style="1" customWidth="1"/>
     <col min="17" max="17" width="30" style="3" customWidth="1"/>
@@ -1003,64 +876,64 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="4" t="s">
+      <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="H1" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="I1" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="J1" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="K1" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="L1" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="4" t="s">
+      <c r="M1" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="4" t="s">
+      <c r="N1" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="4" t="s">
+      <c r="O1" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="4" t="s">
+      <c r="P1" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="4" t="s">
+      <c r="Q1" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="4" t="s">
+      <c r="R1" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="T1" s="4" t="s">
+      <c r="S1" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="T1" s="5" t="s">
         <v>19</v>
       </c>
     </row>
@@ -1081,7 +954,7 @@
         <v>24</v>
       </c>
       <c r="F2" s="1">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="G2" s="1">
         <v>1700</v>
@@ -1090,7 +963,7 @@
         <v>1700</v>
       </c>
       <c r="I2" s="1">
-        <v>0</v>
+        <v>1700</v>
       </c>
       <c r="J2" s="2">
         <v>20536</v>
@@ -1101,10 +974,10 @@
       <c r="L2" s="3">
         <v>5</v>
       </c>
-      <c r="M2" s="2">
-        <v>0</v>
-      </c>
-      <c r="N2" s="2">
+      <c r="M2" s="4">
+        <v>5.7</v>
+      </c>
+      <c r="N2" s="4">
         <v>0</v>
       </c>
       <c r="O2" t="s">
@@ -1143,7 +1016,7 @@
         <v>23</v>
       </c>
       <c r="F3" s="1">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="G3" s="1">
         <v>12800</v>
@@ -1152,7 +1025,7 @@
         <v>12800</v>
       </c>
       <c r="I3" s="1">
-        <v>0</v>
+        <v>12800</v>
       </c>
       <c r="J3" s="2">
         <v>104448</v>
@@ -1163,10 +1036,10 @@
       <c r="L3" s="3">
         <v>8.5</v>
       </c>
-      <c r="M3" s="2">
-        <v>24.66</v>
-      </c>
-      <c r="N3" s="2">
+      <c r="M3" s="4">
+        <v>73.98</v>
+      </c>
+      <c r="N3" s="4">
         <v>0</v>
       </c>
       <c r="O3" t="s">
@@ -1205,7 +1078,7 @@
         <v>23</v>
       </c>
       <c r="F4" s="1">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="G4" s="1">
         <v>4200</v>
@@ -1214,7 +1087,7 @@
         <v>4200</v>
       </c>
       <c r="I4" s="1">
-        <v>0</v>
+        <v>4200</v>
       </c>
       <c r="J4" s="2">
         <v>95760</v>
@@ -1225,10 +1098,10 @@
       <c r="L4" s="3">
         <v>8.5</v>
       </c>
-      <c r="M4" s="2">
-        <v>22.61</v>
-      </c>
-      <c r="N4" s="2">
+      <c r="M4" s="4">
+        <v>67.83</v>
+      </c>
+      <c r="N4" s="4">
         <v>0</v>
       </c>
       <c r="O4" t="s">
@@ -1267,7 +1140,7 @@
         <v>23</v>
       </c>
       <c r="F5" s="1">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="G5" s="1">
         <v>1200</v>
@@ -1276,7 +1149,7 @@
         <v>1200</v>
       </c>
       <c r="I5" s="1">
-        <v>0</v>
+        <v>1200</v>
       </c>
       <c r="J5" s="2">
         <v>94560</v>
@@ -1287,10 +1160,10 @@
       <c r="L5" s="3">
         <v>8.5</v>
       </c>
-      <c r="M5" s="2">
-        <v>22.33</v>
-      </c>
-      <c r="N5" s="2">
+      <c r="M5" s="4">
+        <v>66.98</v>
+      </c>
+      <c r="N5" s="4">
         <v>0</v>
       </c>
       <c r="O5" t="s">
@@ -1329,7 +1202,7 @@
         <v>43</v>
       </c>
       <c r="F6" s="1">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="G6" s="1">
         <v>1600</v>
@@ -1338,7 +1211,7 @@
         <v>1600</v>
       </c>
       <c r="I6" s="1">
-        <v>0</v>
+        <v>1600</v>
       </c>
       <c r="J6" s="2">
         <v>56896</v>
@@ -1349,10 +1222,10 @@
       <c r="L6" s="3">
         <v>8.5</v>
       </c>
-      <c r="M6" s="2">
-        <v>13.43</v>
-      </c>
-      <c r="N6" s="2">
+      <c r="M6" s="4">
+        <v>40.3</v>
+      </c>
+      <c r="N6" s="4">
         <v>0</v>
       </c>
       <c r="O6" t="s">
@@ -1391,7 +1264,7 @@
         <v>43</v>
       </c>
       <c r="F7" s="1">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="G7" s="1">
         <v>3500</v>
@@ -1400,7 +1273,7 @@
         <v>3500</v>
       </c>
       <c r="I7" s="1">
-        <v>0</v>
+        <v>3500</v>
       </c>
       <c r="J7" s="2">
         <v>21805</v>
@@ -1411,10 +1284,10 @@
       <c r="L7" s="3">
         <v>9</v>
       </c>
-      <c r="M7" s="2">
-        <v>5.45</v>
-      </c>
-      <c r="N7" s="2">
+      <c r="M7" s="4">
+        <v>16.35</v>
+      </c>
+      <c r="N7" s="4">
         <v>0</v>
       </c>
       <c r="O7" t="s">
@@ -1453,7 +1326,7 @@
         <v>43</v>
       </c>
       <c r="F8" s="1">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="G8" s="1">
         <v>19200</v>
@@ -1462,7 +1335,7 @@
         <v>19200</v>
       </c>
       <c r="I8" s="1">
-        <v>0</v>
+        <v>19200</v>
       </c>
       <c r="J8" s="2">
         <v>204288</v>
@@ -1473,10 +1346,10 @@
       <c r="L8" s="3">
         <v>9</v>
       </c>
-      <c r="M8" s="2">
-        <v>51.07</v>
-      </c>
-      <c r="N8" s="2">
+      <c r="M8" s="4">
+        <v>153.22</v>
+      </c>
+      <c r="N8" s="4">
         <v>0</v>
       </c>
       <c r="O8" t="s">
@@ -1515,7 +1388,7 @@
         <v>53</v>
       </c>
       <c r="F9" s="1">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="G9" s="1">
         <v>1000</v>
@@ -1524,7 +1397,7 @@
         <v>1000</v>
       </c>
       <c r="I9" s="1">
-        <v>0</v>
+        <v>1000</v>
       </c>
       <c r="J9" s="2">
         <v>5960</v>
@@ -1535,10 +1408,10 @@
       <c r="L9" s="3">
         <v>9</v>
       </c>
-      <c r="M9" s="2">
-        <v>1.49</v>
-      </c>
-      <c r="N9" s="2">
+      <c r="M9" s="4">
+        <v>4.47</v>
+      </c>
+      <c r="N9" s="4">
         <v>0</v>
       </c>
       <c r="O9" t="s">
@@ -1577,7 +1450,7 @@
         <v>24</v>
       </c>
       <c r="F10" s="1">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="G10" s="1">
         <v>1000</v>
@@ -1586,7 +1459,7 @@
         <v>1000</v>
       </c>
       <c r="I10" s="1">
-        <v>0</v>
+        <v>1000</v>
       </c>
       <c r="J10" s="2">
         <v>12080</v>
@@ -1597,10 +1470,10 @@
       <c r="L10" s="3">
         <v>9</v>
       </c>
-      <c r="M10" s="2">
-        <v>3.02</v>
-      </c>
-      <c r="N10" s="2">
+      <c r="M10" s="4">
+        <v>9.06</v>
+      </c>
+      <c r="N10" s="4">
         <v>0</v>
       </c>
       <c r="O10" t="s">
@@ -1639,7 +1512,7 @@
         <v>59</v>
       </c>
       <c r="F11" s="1">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="G11" s="1">
         <v>24500</v>
@@ -1659,10 +1532,10 @@
       <c r="L11" s="3">
         <v>7</v>
       </c>
-      <c r="M11" s="2">
-        <v>35.35</v>
-      </c>
-      <c r="N11" s="2">
+      <c r="M11" s="4">
+        <v>106.04</v>
+      </c>
+      <c r="N11" s="4">
         <v>0</v>
       </c>
       <c r="O11" t="s">
@@ -1701,7 +1574,7 @@
         <v>43</v>
       </c>
       <c r="F12" s="1">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="G12" s="1">
         <v>1900</v>
@@ -1721,10 +1594,10 @@
       <c r="L12" s="3">
         <v>5</v>
       </c>
-      <c r="M12" s="2">
-        <v>2.38</v>
-      </c>
-      <c r="N12" s="2">
+      <c r="M12" s="4">
+        <v>7.15</v>
+      </c>
+      <c r="N12" s="4">
         <v>0</v>
       </c>
       <c r="O12" t="s">
@@ -1763,7 +1636,7 @@
         <v>68</v>
       </c>
       <c r="F13" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G13" s="1">
         <v>16300</v>
@@ -1772,7 +1645,7 @@
         <v>16300</v>
       </c>
       <c r="I13" s="1">
-        <v>16300</v>
+        <v>0</v>
       </c>
       <c r="J13" s="2">
         <v>201957</v>
@@ -1783,10 +1656,10 @@
       <c r="L13" s="3">
         <v>9</v>
       </c>
-      <c r="M13" s="2">
-        <v>201.96</v>
-      </c>
-      <c r="N13" s="2">
+      <c r="M13" s="4">
+        <v>302.94</v>
+      </c>
+      <c r="N13" s="4">
         <v>0</v>
       </c>
       <c r="O13" t="s">
@@ -1825,7 +1698,7 @@
         <v>73</v>
       </c>
       <c r="F14" s="1">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="G14" s="1">
         <v>16600</v>
@@ -1845,10 +1718,10 @@
       <c r="L14" s="3">
         <v>9</v>
       </c>
-      <c r="M14" s="2">
-        <v>197.04</v>
-      </c>
-      <c r="N14" s="2">
+      <c r="M14" s="4">
+        <v>295.56</v>
+      </c>
+      <c r="N14" s="4">
         <v>0</v>
       </c>
       <c r="O14" t="s">
@@ -1887,7 +1760,7 @@
         <v>77</v>
       </c>
       <c r="F15" s="1">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="G15" s="1">
         <v>5000</v>
@@ -1907,10 +1780,10 @@
       <c r="L15" s="3">
         <v>9</v>
       </c>
-      <c r="M15" s="2">
-        <v>59.25</v>
-      </c>
-      <c r="N15" s="2">
+      <c r="M15" s="4">
+        <v>88.88</v>
+      </c>
+      <c r="N15" s="4">
         <v>0</v>
       </c>
       <c r="O15" t="s">
@@ -1943,36 +1816,36 @@
         <v>81</v>
       </c>
       <c r="D16" t="s">
-        <v>22</v>
+        <v>42</v>
       </c>
       <c r="E16" t="s">
-        <v>67</v>
+        <v>77</v>
       </c>
       <c r="F16" s="1">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="G16" s="1">
-        <v>10000</v>
+        <v>9100</v>
       </c>
       <c r="H16" s="1">
-        <v>10000</v>
+        <v>9100</v>
       </c>
       <c r="I16" s="1">
-        <v>10000</v>
+        <v>9100</v>
       </c>
       <c r="J16" s="2">
-        <v>59600</v>
+        <v>59059</v>
       </c>
       <c r="K16" s="3">
         <v>0</v>
       </c>
       <c r="L16" s="3">
-        <v>9</v>
-      </c>
-      <c r="M16" s="2">
-        <v>74.5</v>
-      </c>
-      <c r="N16" s="2">
+        <v>8.5</v>
+      </c>
+      <c r="M16" s="4">
+        <v>97.61</v>
+      </c>
+      <c r="N16" s="4">
         <v>0</v>
       </c>
       <c r="O16" t="s">
@@ -2005,36 +1878,36 @@
         <v>81</v>
       </c>
       <c r="D17" t="s">
-        <v>42</v>
+        <v>85</v>
       </c>
       <c r="E17" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="F17" s="1">
+        <v>20</v>
+      </c>
+      <c r="G17" s="1">
+        <v>1900</v>
+      </c>
+      <c r="H17" s="1">
+        <v>1900</v>
+      </c>
+      <c r="I17" s="1">
+        <v>1900</v>
+      </c>
+      <c r="J17" s="2">
+        <v>191615</v>
+      </c>
+      <c r="K17" s="3">
+        <v>0</v>
+      </c>
+      <c r="L17" s="3">
         <v>9</v>
       </c>
-      <c r="G17" s="1">
-        <v>9100</v>
-      </c>
-      <c r="H17" s="1">
-        <v>9100</v>
-      </c>
-      <c r="I17" s="1">
-        <v>9100</v>
-      </c>
-      <c r="J17" s="2">
-        <v>59059</v>
-      </c>
-      <c r="K17" s="3">
-        <v>0</v>
-      </c>
-      <c r="L17" s="3">
-        <v>8.5</v>
-      </c>
-      <c r="M17" s="2">
-        <v>69.72</v>
-      </c>
-      <c r="N17" s="2">
+      <c r="M17" s="4">
+        <v>335.33</v>
+      </c>
+      <c r="N17" s="4">
         <v>0</v>
       </c>
       <c r="O17" t="s">
@@ -2047,7 +1920,7 @@
         <v>18</v>
       </c>
       <c r="R17" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="S17" t="s">
         <v>27</v>
@@ -2058,58 +1931,58 @@
     </row>
     <row r="18" spans="1:20">
       <c r="A18" t="s">
-        <v>86</v>
+        <v>20</v>
       </c>
       <c r="B18" t="s">
-        <v>87</v>
+        <v>21</v>
       </c>
       <c r="C18" t="s">
         <v>81</v>
       </c>
       <c r="D18" t="s">
+        <v>42</v>
+      </c>
+      <c r="E18" t="s">
+        <v>87</v>
+      </c>
+      <c r="F18" s="1">
+        <v>13</v>
+      </c>
+      <c r="G18" s="1">
+        <v>13900</v>
+      </c>
+      <c r="H18" s="1">
+        <v>13900</v>
+      </c>
+      <c r="I18" s="1">
+        <v>13900</v>
+      </c>
+      <c r="J18" s="2">
+        <v>181117</v>
+      </c>
+      <c r="K18" s="3">
+        <v>0</v>
+      </c>
+      <c r="L18" s="3">
+        <v>5</v>
+      </c>
+      <c r="M18" s="4">
+        <v>176.09</v>
+      </c>
+      <c r="N18" s="4">
+        <v>0</v>
+      </c>
+      <c r="O18" t="s">
+        <v>25</v>
+      </c>
+      <c r="P18" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q18" s="3">
+        <v>18</v>
+      </c>
+      <c r="R18" t="s">
         <v>88</v>
-      </c>
-      <c r="E18" t="s">
-        <v>72</v>
-      </c>
-      <c r="F18" s="1">
-        <v>22</v>
-      </c>
-      <c r="G18" s="1">
-        <v>1900</v>
-      </c>
-      <c r="H18" s="1">
-        <v>1900</v>
-      </c>
-      <c r="I18" s="1">
-        <v>1900</v>
-      </c>
-      <c r="J18" s="2">
-        <v>191615</v>
-      </c>
-      <c r="K18" s="3">
-        <v>0</v>
-      </c>
-      <c r="L18" s="3">
-        <v>9</v>
-      </c>
-      <c r="M18" s="2">
-        <v>239.52</v>
-      </c>
-      <c r="N18" s="2">
-        <v>0</v>
-      </c>
-      <c r="O18" t="s">
-        <v>25</v>
-      </c>
-      <c r="P18" s="1">
-        <v>0</v>
-      </c>
-      <c r="Q18" s="3">
-        <v>18</v>
-      </c>
-      <c r="R18" t="s">
-        <v>89</v>
       </c>
       <c r="S18" t="s">
         <v>27</v>
@@ -2120,10 +1993,10 @@
     </row>
     <row r="19" spans="1:20">
       <c r="A19" t="s">
-        <v>20</v>
+        <v>89</v>
       </c>
       <c r="B19" t="s">
-        <v>21</v>
+        <v>90</v>
       </c>
       <c r="C19" t="s">
         <v>81</v>
@@ -2132,33 +2005,33 @@
         <v>42</v>
       </c>
       <c r="E19" t="s">
-        <v>90</v>
+        <v>53</v>
       </c>
       <c r="F19" s="1">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G19" s="1">
-        <v>13900</v>
+        <v>5400</v>
       </c>
       <c r="H19" s="1">
-        <v>13900</v>
+        <v>5400</v>
       </c>
       <c r="I19" s="1">
-        <v>13900</v>
+        <v>5400</v>
       </c>
       <c r="J19" s="2">
-        <v>181117</v>
+        <v>195480</v>
       </c>
       <c r="K19" s="3">
         <v>0</v>
       </c>
       <c r="L19" s="3">
-        <v>5</v>
-      </c>
-      <c r="M19" s="2">
-        <v>125.78</v>
-      </c>
-      <c r="N19" s="2">
+        <v>7</v>
+      </c>
+      <c r="M19" s="4">
+        <v>266.07</v>
+      </c>
+      <c r="N19" s="4">
         <v>0</v>
       </c>
       <c r="O19" t="s">
@@ -2191,25 +2064,25 @@
         <v>81</v>
       </c>
       <c r="D20" t="s">
-        <v>42</v>
+        <v>94</v>
       </c>
       <c r="E20" t="s">
-        <v>53</v>
+        <v>95</v>
       </c>
       <c r="F20" s="1">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="G20" s="1">
-        <v>5400</v>
+        <v>1800</v>
       </c>
       <c r="H20" s="1">
-        <v>5400</v>
+        <v>1800</v>
       </c>
       <c r="I20" s="1">
-        <v>5400</v>
+        <v>1800</v>
       </c>
       <c r="J20" s="2">
-        <v>195480</v>
+        <v>196200</v>
       </c>
       <c r="K20" s="3">
         <v>0</v>
@@ -2217,10 +2090,10 @@
       <c r="L20" s="3">
         <v>7</v>
       </c>
-      <c r="M20" s="2">
-        <v>190.05</v>
-      </c>
-      <c r="N20" s="2">
+      <c r="M20" s="4">
+        <v>267.05</v>
+      </c>
+      <c r="N20" s="4">
         <v>0</v>
       </c>
       <c r="O20" t="s">
@@ -2233,7 +2106,7 @@
         <v>18</v>
       </c>
       <c r="R20" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="S20" t="s">
         <v>27</v>
@@ -2244,58 +2117,58 @@
     </row>
     <row r="21" spans="1:20">
       <c r="A21" t="s">
-        <v>95</v>
+        <v>61</v>
       </c>
       <c r="B21" t="s">
-        <v>96</v>
+        <v>62</v>
       </c>
       <c r="C21" t="s">
         <v>81</v>
       </c>
       <c r="D21" t="s">
+        <v>42</v>
+      </c>
+      <c r="E21" t="s">
         <v>97</v>
       </c>
-      <c r="E21" t="s">
+      <c r="F21" s="1">
+        <v>8</v>
+      </c>
+      <c r="G21" s="1">
+        <v>15000</v>
+      </c>
+      <c r="H21" s="1">
+        <v>15000</v>
+      </c>
+      <c r="I21" s="1">
+        <v>15000</v>
+      </c>
+      <c r="J21" s="2">
+        <v>133200</v>
+      </c>
+      <c r="K21" s="3">
+        <v>0</v>
+      </c>
+      <c r="L21" s="3">
+        <v>5</v>
+      </c>
+      <c r="M21" s="4">
+        <v>129.5</v>
+      </c>
+      <c r="N21" s="4">
+        <v>0</v>
+      </c>
+      <c r="O21" t="s">
+        <v>25</v>
+      </c>
+      <c r="P21" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q21" s="3">
+        <v>18</v>
+      </c>
+      <c r="R21" t="s">
         <v>98</v>
-      </c>
-      <c r="F21" s="1">
-        <v>20</v>
-      </c>
-      <c r="G21" s="1">
-        <v>1800</v>
-      </c>
-      <c r="H21" s="1">
-        <v>1800</v>
-      </c>
-      <c r="I21" s="1">
-        <v>1800</v>
-      </c>
-      <c r="J21" s="2">
-        <v>196200</v>
-      </c>
-      <c r="K21" s="3">
-        <v>0</v>
-      </c>
-      <c r="L21" s="3">
-        <v>7</v>
-      </c>
-      <c r="M21" s="2">
-        <v>190.75</v>
-      </c>
-      <c r="N21" s="2">
-        <v>0</v>
-      </c>
-      <c r="O21" t="s">
-        <v>25</v>
-      </c>
-      <c r="P21" s="1">
-        <v>0</v>
-      </c>
-      <c r="Q21" s="3">
-        <v>18</v>
-      </c>
-      <c r="R21" t="s">
-        <v>99</v>
       </c>
       <c r="S21" t="s">
         <v>27</v>
@@ -2306,10 +2179,10 @@
     </row>
     <row r="22" spans="1:20">
       <c r="A22" t="s">
-        <v>61</v>
+        <v>45</v>
       </c>
       <c r="B22" t="s">
-        <v>62</v>
+        <v>46</v>
       </c>
       <c r="C22" t="s">
         <v>81</v>
@@ -2318,22 +2191,22 @@
         <v>42</v>
       </c>
       <c r="E22" t="s">
-        <v>100</v>
+        <v>43</v>
       </c>
       <c r="F22" s="1">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G22" s="1">
-        <v>15000</v>
+        <v>28900</v>
       </c>
       <c r="H22" s="1">
-        <v>15000</v>
+        <v>28900</v>
       </c>
       <c r="I22" s="1">
-        <v>15000</v>
+        <v>28900</v>
       </c>
       <c r="J22" s="2">
-        <v>133200</v>
+        <v>184382</v>
       </c>
       <c r="K22" s="3">
         <v>0</v>
@@ -2341,10 +2214,10 @@
       <c r="L22" s="3">
         <v>5</v>
       </c>
-      <c r="M22" s="2">
-        <v>92.5</v>
-      </c>
-      <c r="N22" s="2">
+      <c r="M22" s="4">
+        <v>179.26</v>
+      </c>
+      <c r="N22" s="4">
         <v>0</v>
       </c>
       <c r="O22" t="s">
@@ -2357,7 +2230,7 @@
         <v>18</v>
       </c>
       <c r="R22" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="S22" t="s">
         <v>27</v>
@@ -2368,34 +2241,34 @@
     </row>
     <row r="23" spans="1:20">
       <c r="A23" t="s">
-        <v>45</v>
+        <v>61</v>
       </c>
       <c r="B23" t="s">
-        <v>46</v>
+        <v>62</v>
       </c>
       <c r="C23" t="s">
         <v>81</v>
       </c>
       <c r="D23" t="s">
-        <v>42</v>
+        <v>59</v>
       </c>
       <c r="E23" t="s">
-        <v>43</v>
+        <v>100</v>
       </c>
       <c r="F23" s="1">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="G23" s="1">
-        <v>28900</v>
+        <v>6400</v>
       </c>
       <c r="H23" s="1">
-        <v>28900</v>
+        <v>6400</v>
       </c>
       <c r="I23" s="1">
-        <v>28900</v>
+        <v>6400</v>
       </c>
       <c r="J23" s="2">
-        <v>184382</v>
+        <v>56832</v>
       </c>
       <c r="K23" s="3">
         <v>0</v>
@@ -2403,10 +2276,10 @@
       <c r="L23" s="3">
         <v>5</v>
       </c>
-      <c r="M23" s="2">
-        <v>128.04</v>
-      </c>
-      <c r="N23" s="2">
+      <c r="M23" s="4">
+        <v>55.25</v>
+      </c>
+      <c r="N23" s="4">
         <v>0</v>
       </c>
       <c r="O23" t="s">
@@ -2419,7 +2292,7 @@
         <v>18</v>
       </c>
       <c r="R23" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="S23" t="s">
         <v>27</v>
@@ -2430,45 +2303,45 @@
     </row>
     <row r="24" spans="1:20">
       <c r="A24" t="s">
-        <v>61</v>
+        <v>102</v>
       </c>
       <c r="B24" t="s">
-        <v>62</v>
+        <v>103</v>
       </c>
       <c r="C24" t="s">
         <v>81</v>
       </c>
       <c r="D24" t="s">
-        <v>59</v>
+        <v>100</v>
       </c>
       <c r="E24" t="s">
-        <v>103</v>
+        <v>42</v>
       </c>
       <c r="F24" s="1">
+        <v>6</v>
+      </c>
+      <c r="G24" s="1">
+        <v>1300</v>
+      </c>
+      <c r="H24" s="1">
+        <v>1300</v>
+      </c>
+      <c r="I24" s="1">
+        <v>1300</v>
+      </c>
+      <c r="J24" s="2">
+        <v>86320</v>
+      </c>
+      <c r="K24" s="3">
+        <v>0</v>
+      </c>
+      <c r="L24" s="3">
         <v>7</v>
       </c>
-      <c r="G24" s="1">
-        <v>6400</v>
-      </c>
-      <c r="H24" s="1">
-        <v>6400</v>
-      </c>
-      <c r="I24" s="1">
-        <v>6400</v>
-      </c>
-      <c r="J24" s="2">
-        <v>56832</v>
-      </c>
-      <c r="K24" s="3">
-        <v>0</v>
-      </c>
-      <c r="L24" s="3">
-        <v>5</v>
-      </c>
-      <c r="M24" s="2">
-        <v>39.47</v>
-      </c>
-      <c r="N24" s="2">
+      <c r="M24" s="4">
+        <v>117.49</v>
+      </c>
+      <c r="N24" s="4">
         <v>0</v>
       </c>
       <c r="O24" t="s">
@@ -2501,25 +2374,25 @@
         <v>81</v>
       </c>
       <c r="D25" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="E25" t="s">
         <v>42</v>
       </c>
       <c r="F25" s="1">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G25" s="1">
-        <v>1300</v>
+        <v>11700</v>
       </c>
       <c r="H25" s="1">
-        <v>1300</v>
+        <v>11700</v>
       </c>
       <c r="I25" s="1">
-        <v>1300</v>
+        <v>11700</v>
       </c>
       <c r="J25" s="2">
-        <v>86320</v>
+        <v>96993</v>
       </c>
       <c r="K25" s="3">
         <v>0</v>
@@ -2527,10 +2400,10 @@
       <c r="L25" s="3">
         <v>7</v>
       </c>
-      <c r="M25" s="2">
-        <v>83.92</v>
-      </c>
-      <c r="N25" s="2">
+      <c r="M25" s="4">
+        <v>132.02</v>
+      </c>
+      <c r="N25" s="4">
         <v>0</v>
       </c>
       <c r="O25" t="s">
@@ -2563,25 +2436,25 @@
         <v>81</v>
       </c>
       <c r="D26" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="E26" t="s">
         <v>42</v>
       </c>
       <c r="F26" s="1">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G26" s="1">
-        <v>11700</v>
+        <v>7000</v>
       </c>
       <c r="H26" s="1">
-        <v>11700</v>
+        <v>7000</v>
       </c>
       <c r="I26" s="1">
-        <v>11700</v>
+        <v>7000</v>
       </c>
       <c r="J26" s="2">
-        <v>96993</v>
+        <v>95970</v>
       </c>
       <c r="K26" s="3">
         <v>0</v>
@@ -2589,10 +2462,10 @@
       <c r="L26" s="3">
         <v>7</v>
       </c>
-      <c r="M26" s="2">
-        <v>94.3</v>
-      </c>
-      <c r="N26" s="2">
+      <c r="M26" s="4">
+        <v>130.63</v>
+      </c>
+      <c r="N26" s="4">
         <v>0</v>
       </c>
       <c r="O26" t="s">
@@ -2616,45 +2489,45 @@
     </row>
     <row r="27" spans="1:20">
       <c r="A27" t="s">
+        <v>108</v>
+      </c>
+      <c r="B27" t="s">
+        <v>109</v>
+      </c>
+      <c r="C27" t="s">
         <v>111</v>
       </c>
-      <c r="B27" t="s">
-        <v>112</v>
-      </c>
-      <c r="C27" t="s">
-        <v>81</v>
-      </c>
       <c r="D27" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="E27" t="s">
         <v>42</v>
       </c>
       <c r="F27" s="1">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G27" s="1">
-        <v>7000</v>
+        <v>6600</v>
       </c>
       <c r="H27" s="1">
-        <v>7000</v>
+        <v>6600</v>
       </c>
       <c r="I27" s="1">
-        <v>7000</v>
+        <v>6600</v>
       </c>
       <c r="J27" s="2">
-        <v>95970</v>
+        <v>97482</v>
       </c>
       <c r="K27" s="3">
         <v>0</v>
       </c>
       <c r="L27" s="3">
-        <v>7</v>
-      </c>
-      <c r="M27" s="2">
-        <v>93.3</v>
-      </c>
-      <c r="N27" s="2">
+        <v>8.5</v>
+      </c>
+      <c r="M27" s="4">
+        <v>184.13</v>
+      </c>
+      <c r="N27" s="4">
         <v>0</v>
       </c>
       <c r="O27" t="s">
@@ -2667,7 +2540,7 @@
         <v>18</v>
       </c>
       <c r="R27" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="S27" t="s">
         <v>27</v>
@@ -2678,34 +2551,34 @@
     </row>
     <row r="28" spans="1:20">
       <c r="A28" t="s">
+        <v>105</v>
+      </c>
+      <c r="B28" t="s">
+        <v>106</v>
+      </c>
+      <c r="C28" t="s">
         <v>111</v>
       </c>
-      <c r="B28" t="s">
-        <v>112</v>
-      </c>
-      <c r="C28" t="s">
-        <v>114</v>
-      </c>
       <c r="D28" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="E28" t="s">
         <v>42</v>
       </c>
       <c r="F28" s="1">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G28" s="1">
-        <v>6600</v>
+        <v>11600</v>
       </c>
       <c r="H28" s="1">
-        <v>6600</v>
+        <v>11600</v>
       </c>
       <c r="I28" s="1">
-        <v>6600</v>
+        <v>11600</v>
       </c>
       <c r="J28" s="2">
-        <v>97482</v>
+        <v>99644</v>
       </c>
       <c r="K28" s="3">
         <v>0</v>
@@ -2713,10 +2586,10 @@
       <c r="L28" s="3">
         <v>8.5</v>
       </c>
-      <c r="M28" s="2">
-        <v>138.1</v>
-      </c>
-      <c r="N28" s="2">
+      <c r="M28" s="4">
+        <v>188.22</v>
+      </c>
+      <c r="N28" s="4">
         <v>0</v>
       </c>
       <c r="O28" t="s">
@@ -2729,7 +2602,7 @@
         <v>18</v>
       </c>
       <c r="R28" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="S28" t="s">
         <v>27</v>
@@ -2740,34 +2613,34 @@
     </row>
     <row r="29" spans="1:20">
       <c r="A29" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="B29" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="C29" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="D29" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="E29" t="s">
         <v>42</v>
       </c>
       <c r="F29" s="1">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G29" s="1">
-        <v>11600</v>
+        <v>1600</v>
       </c>
       <c r="H29" s="1">
-        <v>11600</v>
+        <v>1600</v>
       </c>
       <c r="I29" s="1">
-        <v>11600</v>
+        <v>1600</v>
       </c>
       <c r="J29" s="2">
-        <v>99644</v>
+        <v>110992</v>
       </c>
       <c r="K29" s="3">
         <v>0</v>
@@ -2775,10 +2648,10 @@
       <c r="L29" s="3">
         <v>8.5</v>
       </c>
-      <c r="M29" s="2">
-        <v>141.16</v>
-      </c>
-      <c r="N29" s="2">
+      <c r="M29" s="4">
+        <v>209.65</v>
+      </c>
+      <c r="N29" s="4">
         <v>0</v>
       </c>
       <c r="O29" t="s">
@@ -2791,7 +2664,7 @@
         <v>18</v>
       </c>
       <c r="R29" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="S29" t="s">
         <v>27</v>
@@ -2802,45 +2675,45 @@
     </row>
     <row r="30" spans="1:20">
       <c r="A30" t="s">
-        <v>105</v>
+        <v>115</v>
       </c>
       <c r="B30" t="s">
-        <v>106</v>
+        <v>116</v>
       </c>
       <c r="C30" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="D30" t="s">
-        <v>103</v>
+        <v>58</v>
       </c>
       <c r="E30" t="s">
-        <v>42</v>
+        <v>59</v>
       </c>
       <c r="F30" s="1">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="G30" s="1">
-        <v>1600</v>
+        <v>1000</v>
       </c>
       <c r="H30" s="1">
-        <v>1600</v>
+        <v>1000</v>
       </c>
       <c r="I30" s="1">
-        <v>1600</v>
+        <v>1000</v>
       </c>
       <c r="J30" s="2">
-        <v>110992</v>
+        <v>15550</v>
       </c>
       <c r="K30" s="3">
         <v>0</v>
       </c>
       <c r="L30" s="3">
-        <v>8.5</v>
-      </c>
-      <c r="M30" s="2">
-        <v>157.24</v>
-      </c>
-      <c r="N30" s="2">
+        <v>9</v>
+      </c>
+      <c r="M30" s="4">
+        <v>31.1</v>
+      </c>
+      <c r="N30" s="4">
         <v>0</v>
       </c>
       <c r="O30" t="s">
@@ -2864,58 +2737,58 @@
     </row>
     <row r="31" spans="1:20">
       <c r="A31" t="s">
+        <v>92</v>
+      </c>
+      <c r="B31" t="s">
+        <v>93</v>
+      </c>
+      <c r="C31" t="s">
+        <v>111</v>
+      </c>
+      <c r="D31" t="s">
+        <v>94</v>
+      </c>
+      <c r="E31" t="s">
+        <v>95</v>
+      </c>
+      <c r="F31" s="1">
+        <v>18</v>
+      </c>
+      <c r="G31" s="1">
+        <v>1900</v>
+      </c>
+      <c r="H31" s="1">
+        <v>1900</v>
+      </c>
+      <c r="I31" s="1">
+        <v>1900</v>
+      </c>
+      <c r="J31" s="2">
+        <v>216277</v>
+      </c>
+      <c r="K31" s="3">
+        <v>0</v>
+      </c>
+      <c r="L31" s="3">
+        <v>7</v>
+      </c>
+      <c r="M31" s="4">
+        <v>336.43</v>
+      </c>
+      <c r="N31" s="4">
+        <v>0</v>
+      </c>
+      <c r="O31" t="s">
+        <v>25</v>
+      </c>
+      <c r="P31" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q31" s="3">
+        <v>18</v>
+      </c>
+      <c r="R31" t="s">
         <v>118</v>
-      </c>
-      <c r="B31" t="s">
-        <v>119</v>
-      </c>
-      <c r="C31" t="s">
-        <v>114</v>
-      </c>
-      <c r="D31" t="s">
-        <v>58</v>
-      </c>
-      <c r="E31" t="s">
-        <v>59</v>
-      </c>
-      <c r="F31" s="1">
-        <v>6</v>
-      </c>
-      <c r="G31" s="1">
-        <v>1000</v>
-      </c>
-      <c r="H31" s="1">
-        <v>1000</v>
-      </c>
-      <c r="I31" s="1">
-        <v>1000</v>
-      </c>
-      <c r="J31" s="2">
-        <v>15550</v>
-      </c>
-      <c r="K31" s="3">
-        <v>0</v>
-      </c>
-      <c r="L31" s="3">
-        <v>9</v>
-      </c>
-      <c r="M31" s="2">
-        <v>23.32</v>
-      </c>
-      <c r="N31" s="2">
-        <v>0</v>
-      </c>
-      <c r="O31" t="s">
-        <v>25</v>
-      </c>
-      <c r="P31" s="1">
-        <v>0</v>
-      </c>
-      <c r="Q31" s="3">
-        <v>18</v>
-      </c>
-      <c r="R31" t="s">
-        <v>120</v>
       </c>
       <c r="S31" t="s">
         <v>27</v>
@@ -2926,34 +2799,34 @@
     </row>
     <row r="32" spans="1:20">
       <c r="A32" t="s">
-        <v>95</v>
+        <v>56</v>
       </c>
       <c r="B32" t="s">
-        <v>96</v>
+        <v>57</v>
       </c>
       <c r="C32" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="D32" t="s">
-        <v>97</v>
+        <v>58</v>
       </c>
       <c r="E32" t="s">
-        <v>98</v>
+        <v>59</v>
       </c>
       <c r="F32" s="1">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="G32" s="1">
-        <v>1900</v>
+        <v>1200</v>
       </c>
       <c r="H32" s="1">
-        <v>1900</v>
+        <v>1200</v>
       </c>
       <c r="I32" s="1">
-        <v>1900</v>
+        <v>1200</v>
       </c>
       <c r="J32" s="2">
-        <v>216277</v>
+        <v>9264</v>
       </c>
       <c r="K32" s="3">
         <v>0</v>
@@ -2961,10 +2834,10 @@
       <c r="L32" s="3">
         <v>7</v>
       </c>
-      <c r="M32" s="2">
-        <v>252.32</v>
-      </c>
-      <c r="N32" s="2">
+      <c r="M32" s="4">
+        <v>14.41</v>
+      </c>
+      <c r="N32" s="4">
         <v>0</v>
       </c>
       <c r="O32" t="s">
@@ -2977,7 +2850,7 @@
         <v>18</v>
       </c>
       <c r="R32" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="S32" t="s">
         <v>27</v>
@@ -2988,45 +2861,45 @@
     </row>
     <row r="33" spans="1:20">
       <c r="A33" t="s">
-        <v>56</v>
+        <v>120</v>
       </c>
       <c r="B33" t="s">
-        <v>57</v>
+        <v>121</v>
       </c>
       <c r="C33" t="s">
-        <v>114</v>
+        <v>122</v>
       </c>
       <c r="D33" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="E33" t="s">
-        <v>59</v>
+        <v>100</v>
       </c>
       <c r="F33" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G33" s="1">
-        <v>1200</v>
+        <v>10000</v>
       </c>
       <c r="H33" s="1">
-        <v>1200</v>
+        <v>10000</v>
       </c>
       <c r="I33" s="1">
-        <v>1200</v>
+        <v>10000</v>
       </c>
       <c r="J33" s="2">
-        <v>9264</v>
+        <v>81800</v>
       </c>
       <c r="K33" s="3">
         <v>0</v>
       </c>
       <c r="L33" s="3">
-        <v>7</v>
-      </c>
-      <c r="M33" s="2">
-        <v>10.81</v>
-      </c>
-      <c r="N33" s="2">
+        <v>8.5</v>
+      </c>
+      <c r="M33" s="4">
+        <v>173.83</v>
+      </c>
+      <c r="N33" s="4">
         <v>0</v>
       </c>
       <c r="O33" t="s">
@@ -3039,7 +2912,7 @@
         <v>18</v>
       </c>
       <c r="R33" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="S33" t="s">
         <v>27</v>
@@ -3050,45 +2923,45 @@
     </row>
     <row r="34" spans="1:20">
       <c r="A34" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="B34" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C34" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="D34" t="s">
         <v>59</v>
       </c>
       <c r="E34" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="F34" s="1">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="G34" s="1">
-        <v>10000</v>
+        <v>400</v>
       </c>
       <c r="H34" s="1">
-        <v>10000</v>
+        <v>400</v>
       </c>
       <c r="I34" s="1">
-        <v>10000</v>
+        <v>400</v>
       </c>
       <c r="J34" s="2">
-        <v>81800</v>
+        <v>3392</v>
       </c>
       <c r="K34" s="3">
         <v>0</v>
       </c>
       <c r="L34" s="3">
-        <v>8.5</v>
-      </c>
-      <c r="M34" s="2">
-        <v>135.2</v>
-      </c>
-      <c r="N34" s="2">
+        <v>9</v>
+      </c>
+      <c r="M34" s="4">
+        <v>7.63</v>
+      </c>
+      <c r="N34" s="4">
         <v>0</v>
       </c>
       <c r="O34" t="s">
@@ -3118,39 +2991,39 @@
         <v>128</v>
       </c>
       <c r="C35" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="D35" t="s">
         <v>59</v>
       </c>
       <c r="E35" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="F35" s="1">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="G35" s="1">
-        <v>400</v>
+        <v>9500</v>
       </c>
       <c r="H35" s="1">
-        <v>400</v>
+        <v>9500</v>
       </c>
       <c r="I35" s="1">
-        <v>400</v>
+        <v>9500</v>
       </c>
       <c r="J35" s="2">
-        <v>3392</v>
+        <v>94620</v>
       </c>
       <c r="K35" s="3">
         <v>0</v>
       </c>
       <c r="L35" s="3">
-        <v>9</v>
-      </c>
-      <c r="M35" s="2">
-        <v>5.94</v>
-      </c>
-      <c r="N35" s="2">
+        <v>8.5</v>
+      </c>
+      <c r="M35" s="4">
+        <v>201.07</v>
+      </c>
+      <c r="N35" s="4">
         <v>0</v>
       </c>
       <c r="O35" t="s">
@@ -3174,45 +3047,45 @@
     </row>
     <row r="36" spans="1:20">
       <c r="A36" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="B36" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="C36" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="D36" t="s">
         <v>59</v>
       </c>
       <c r="E36" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="F36" s="1">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="G36" s="1">
-        <v>9500</v>
+        <v>9800</v>
       </c>
       <c r="H36" s="1">
-        <v>9500</v>
+        <v>9800</v>
       </c>
       <c r="I36" s="1">
-        <v>9500</v>
+        <v>9800</v>
       </c>
       <c r="J36" s="2">
-        <v>94620</v>
+        <v>83104</v>
       </c>
       <c r="K36" s="3">
         <v>0</v>
       </c>
       <c r="L36" s="3">
-        <v>8.5</v>
-      </c>
-      <c r="M36" s="2">
-        <v>156.39</v>
-      </c>
-      <c r="N36" s="2">
+        <v>9</v>
+      </c>
+      <c r="M36" s="4">
+        <v>186.98</v>
+      </c>
+      <c r="N36" s="4">
         <v>0</v>
       </c>
       <c r="O36" t="s">
@@ -3225,7 +3098,7 @@
         <v>18</v>
       </c>
       <c r="R36" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="S36" t="s">
         <v>27</v>
@@ -3236,34 +3109,34 @@
     </row>
     <row r="37" spans="1:20">
       <c r="A37" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="B37" t="s">
-        <v>128</v>
+        <v>132</v>
       </c>
       <c r="C37" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="D37" t="s">
         <v>59</v>
       </c>
       <c r="E37" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="F37" s="1">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="G37" s="1">
-        <v>9800</v>
+        <v>1400</v>
       </c>
       <c r="H37" s="1">
-        <v>9800</v>
+        <v>1400</v>
       </c>
       <c r="I37" s="1">
-        <v>9800</v>
+        <v>1400</v>
       </c>
       <c r="J37" s="2">
-        <v>83104</v>
+        <v>192360</v>
       </c>
       <c r="K37" s="3">
         <v>0</v>
@@ -3271,10 +3144,10 @@
       <c r="L37" s="3">
         <v>9</v>
       </c>
-      <c r="M37" s="2">
-        <v>145.43</v>
-      </c>
-      <c r="N37" s="2">
+      <c r="M37" s="4">
+        <v>432.81</v>
+      </c>
+      <c r="N37" s="4">
         <v>0</v>
       </c>
       <c r="O37" t="s">
@@ -3304,28 +3177,28 @@
         <v>135</v>
       </c>
       <c r="C38" t="s">
-        <v>125</v>
+        <v>136</v>
       </c>
       <c r="D38" t="s">
+        <v>58</v>
+      </c>
+      <c r="E38" t="s">
         <v>59</v>
       </c>
-      <c r="E38" t="s">
-        <v>103</v>
-      </c>
       <c r="F38" s="1">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="G38" s="1">
-        <v>1400</v>
+        <v>22900</v>
       </c>
       <c r="H38" s="1">
-        <v>1400</v>
+        <v>22900</v>
       </c>
       <c r="I38" s="1">
-        <v>1400</v>
+        <v>22900</v>
       </c>
       <c r="J38" s="2">
-        <v>192360</v>
+        <v>210451</v>
       </c>
       <c r="K38" s="3">
         <v>0</v>
@@ -3333,10 +3206,10 @@
       <c r="L38" s="3">
         <v>9</v>
       </c>
-      <c r="M38" s="2">
-        <v>336.63</v>
-      </c>
-      <c r="N38" s="2">
+      <c r="M38" s="4">
+        <v>526.13</v>
+      </c>
+      <c r="N38" s="4">
         <v>0</v>
       </c>
       <c r="O38" t="s">
@@ -3349,7 +3222,7 @@
         <v>18</v>
       </c>
       <c r="R38" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="S38" t="s">
         <v>27</v>
@@ -3360,13 +3233,13 @@
     </row>
     <row r="39" spans="1:20">
       <c r="A39" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="B39" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="C39" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="D39" t="s">
         <v>58</v>
@@ -3375,19 +3248,19 @@
         <v>59</v>
       </c>
       <c r="F39" s="1">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="G39" s="1">
-        <v>22900</v>
+        <v>1200</v>
       </c>
       <c r="H39" s="1">
-        <v>22900</v>
+        <v>1200</v>
       </c>
       <c r="I39" s="1">
-        <v>22900</v>
+        <v>1200</v>
       </c>
       <c r="J39" s="2">
-        <v>210451</v>
+        <v>10188</v>
       </c>
       <c r="K39" s="3">
         <v>0</v>
@@ -3395,10 +3268,10 @@
       <c r="L39" s="3">
         <v>9</v>
       </c>
-      <c r="M39" s="2">
-        <v>420.9</v>
-      </c>
-      <c r="N39" s="2">
+      <c r="M39" s="4">
+        <v>25.47</v>
+      </c>
+      <c r="N39" s="4">
         <v>0</v>
       </c>
       <c r="O39" t="s">
@@ -3428,7 +3301,7 @@
         <v>142</v>
       </c>
       <c r="C40" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="D40" t="s">
         <v>58</v>
@@ -3437,19 +3310,19 @@
         <v>59</v>
       </c>
       <c r="F40" s="1">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="G40" s="1">
-        <v>1200</v>
+        <v>1400</v>
       </c>
       <c r="H40" s="1">
-        <v>1200</v>
+        <v>1400</v>
       </c>
       <c r="I40" s="1">
-        <v>1200</v>
+        <v>1400</v>
       </c>
       <c r="J40" s="2">
-        <v>10188</v>
+        <v>151508</v>
       </c>
       <c r="K40" s="3">
         <v>0</v>
@@ -3457,10 +3330,10 @@
       <c r="L40" s="3">
         <v>9</v>
       </c>
-      <c r="M40" s="2">
-        <v>20.38</v>
-      </c>
-      <c r="N40" s="2">
+      <c r="M40" s="4">
+        <v>378.77</v>
+      </c>
+      <c r="N40" s="4">
         <v>0</v>
       </c>
       <c r="O40" t="s">
@@ -3484,34 +3357,34 @@
     </row>
     <row r="41" spans="1:20">
       <c r="A41" t="s">
+        <v>141</v>
+      </c>
+      <c r="B41" t="s">
+        <v>142</v>
+      </c>
+      <c r="C41" t="s">
         <v>144</v>
       </c>
-      <c r="B41" t="s">
-        <v>145</v>
-      </c>
-      <c r="C41" t="s">
-        <v>139</v>
-      </c>
       <c r="D41" t="s">
-        <v>58</v>
+        <v>42</v>
       </c>
       <c r="E41" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="F41" s="1">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="G41" s="1">
-        <v>1400</v>
+        <v>500</v>
       </c>
       <c r="H41" s="1">
-        <v>1400</v>
+        <v>500</v>
       </c>
       <c r="I41" s="1">
-        <v>1400</v>
+        <v>500</v>
       </c>
       <c r="J41" s="2">
-        <v>151508</v>
+        <v>53655</v>
       </c>
       <c r="K41" s="3">
         <v>0</v>
@@ -3519,10 +3392,10 @@
       <c r="L41" s="3">
         <v>9</v>
       </c>
-      <c r="M41" s="2">
-        <v>303.02</v>
-      </c>
-      <c r="N41" s="2">
+      <c r="M41" s="4">
+        <v>174.38</v>
+      </c>
+      <c r="N41" s="4">
         <v>0</v>
       </c>
       <c r="O41" t="s">
@@ -3535,7 +3408,7 @@
         <v>18</v>
       </c>
       <c r="R41" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="S41" t="s">
         <v>27</v>
@@ -3546,45 +3419,45 @@
     </row>
     <row r="42" spans="1:20">
       <c r="A42" t="s">
+        <v>146</v>
+      </c>
+      <c r="B42" t="s">
         <v>147</v>
       </c>
-      <c r="B42" t="s">
+      <c r="C42" t="s">
         <v>148</v>
       </c>
-      <c r="C42" t="s">
-        <v>139</v>
-      </c>
       <c r="D42" t="s">
-        <v>31</v>
+        <v>67</v>
       </c>
       <c r="E42" t="s">
-        <v>22</v>
+        <v>68</v>
       </c>
       <c r="F42" s="1">
         <v>0</v>
       </c>
       <c r="G42" s="1">
-        <v>16600</v>
+        <v>1600</v>
       </c>
       <c r="H42" s="1">
-        <v>16600</v>
+        <v>1600</v>
       </c>
       <c r="I42" s="1">
         <v>0</v>
       </c>
       <c r="J42" s="2">
-        <v>194552</v>
+        <v>47440</v>
       </c>
       <c r="K42" s="3">
         <v>0</v>
       </c>
       <c r="L42" s="3">
-        <v>9</v>
-      </c>
-      <c r="M42" s="2">
-        <v>389.1</v>
-      </c>
-      <c r="N42" s="2">
+        <v>8.5</v>
+      </c>
+      <c r="M42" s="4">
+        <v>156.82</v>
+      </c>
+      <c r="N42" s="4">
         <v>0</v>
       </c>
       <c r="O42" t="s">
@@ -3608,45 +3481,45 @@
     </row>
     <row r="43" spans="1:20">
       <c r="A43" t="s">
-        <v>144</v>
+        <v>150</v>
       </c>
       <c r="B43" t="s">
-        <v>145</v>
+        <v>151</v>
       </c>
       <c r="C43" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="D43" t="s">
-        <v>42</v>
+        <v>67</v>
       </c>
       <c r="E43" t="s">
-        <v>53</v>
+        <v>68</v>
       </c>
       <c r="F43" s="1">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="G43" s="1">
-        <v>500</v>
+        <v>1200</v>
       </c>
       <c r="H43" s="1">
-        <v>500</v>
+        <v>1200</v>
       </c>
       <c r="I43" s="1">
-        <v>500</v>
+        <v>0</v>
       </c>
       <c r="J43" s="2">
-        <v>53655</v>
+        <v>221280</v>
       </c>
       <c r="K43" s="3">
         <v>0</v>
       </c>
       <c r="L43" s="3">
-        <v>9</v>
-      </c>
-      <c r="M43" s="2">
-        <v>147.55</v>
-      </c>
-      <c r="N43" s="2">
+        <v>8.5</v>
+      </c>
+      <c r="M43" s="4">
+        <v>731.45</v>
+      </c>
+      <c r="N43" s="4">
         <v>0</v>
       </c>
       <c r="O43" t="s">
@@ -3659,7 +3532,7 @@
         <v>18</v>
       </c>
       <c r="R43" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="S43" t="s">
         <v>27</v>
@@ -3670,45 +3543,45 @@
     </row>
     <row r="44" spans="1:20">
       <c r="A44" t="s">
-        <v>152</v>
+        <v>79</v>
       </c>
       <c r="B44" t="s">
+        <v>80</v>
+      </c>
+      <c r="C44" t="s">
         <v>153</v>
       </c>
-      <c r="C44" t="s">
+      <c r="D44" t="s">
+        <v>42</v>
+      </c>
+      <c r="E44" t="s">
         <v>154</v>
       </c>
-      <c r="D44" t="s">
-        <v>67</v>
-      </c>
-      <c r="E44" t="s">
-        <v>68</v>
-      </c>
       <c r="F44" s="1">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="G44" s="1">
-        <v>1600</v>
+        <v>19200</v>
       </c>
       <c r="H44" s="1">
-        <v>1600</v>
+        <v>19200</v>
       </c>
       <c r="I44" s="1">
-        <v>1600</v>
+        <v>19200</v>
       </c>
       <c r="J44" s="2">
-        <v>47440</v>
+        <v>131904</v>
       </c>
       <c r="K44" s="3">
         <v>0</v>
       </c>
       <c r="L44" s="3">
-        <v>8.5</v>
-      </c>
-      <c r="M44" s="2">
-        <v>134.41</v>
-      </c>
-      <c r="N44" s="2">
+        <v>9</v>
+      </c>
+      <c r="M44" s="4">
+        <v>494.64</v>
+      </c>
+      <c r="N44" s="4">
         <v>0</v>
       </c>
       <c r="O44" t="s">
@@ -3738,39 +3611,39 @@
         <v>157</v>
       </c>
       <c r="C45" t="s">
+        <v>153</v>
+      </c>
+      <c r="D45" t="s">
+        <v>42</v>
+      </c>
+      <c r="E45" t="s">
         <v>154</v>
       </c>
-      <c r="D45" t="s">
-        <v>67</v>
-      </c>
-      <c r="E45" t="s">
-        <v>68</v>
-      </c>
       <c r="F45" s="1">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="G45" s="1">
-        <v>1200</v>
+        <v>4200</v>
       </c>
       <c r="H45" s="1">
-        <v>1200</v>
+        <v>4200</v>
       </c>
       <c r="I45" s="1">
-        <v>1200</v>
+        <v>4200</v>
       </c>
       <c r="J45" s="2">
-        <v>221280</v>
+        <v>108360</v>
       </c>
       <c r="K45" s="3">
         <v>0</v>
       </c>
       <c r="L45" s="3">
-        <v>8.5</v>
-      </c>
-      <c r="M45" s="2">
-        <v>626.96</v>
-      </c>
-      <c r="N45" s="2">
+        <v>7</v>
+      </c>
+      <c r="M45" s="4">
+        <v>316.05</v>
+      </c>
+      <c r="N45" s="4">
         <v>0</v>
       </c>
       <c r="O45" t="s">
@@ -3794,34 +3667,34 @@
     </row>
     <row r="46" spans="1:20">
       <c r="A46" t="s">
+        <v>83</v>
+      </c>
+      <c r="B46" t="s">
+        <v>84</v>
+      </c>
+      <c r="C46" t="s">
         <v>159</v>
       </c>
-      <c r="B46" t="s">
-        <v>160</v>
-      </c>
-      <c r="C46" t="s">
-        <v>154</v>
-      </c>
       <c r="D46" t="s">
-        <v>22</v>
+        <v>42</v>
       </c>
       <c r="E46" t="s">
-        <v>67</v>
+        <v>97</v>
       </c>
       <c r="F46" s="1">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="G46" s="1">
-        <v>2300</v>
+        <v>1000</v>
       </c>
       <c r="H46" s="1">
-        <v>2300</v>
+        <v>1000</v>
       </c>
       <c r="I46" s="1">
-        <v>2300</v>
+        <v>1000</v>
       </c>
       <c r="J46" s="2">
-        <v>200491</v>
+        <v>83100</v>
       </c>
       <c r="K46" s="3">
         <v>0</v>
@@ -3829,10 +3702,10 @@
       <c r="L46" s="3">
         <v>9</v>
       </c>
-      <c r="M46" s="2">
-        <v>601.47</v>
-      </c>
-      <c r="N46" s="2">
+      <c r="M46" s="4">
+        <v>353.18</v>
+      </c>
+      <c r="N46" s="4">
         <v>0</v>
       </c>
       <c r="O46" t="s">
@@ -3845,7 +3718,7 @@
         <v>18</v>
       </c>
       <c r="R46" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="S46" t="s">
         <v>27</v>
@@ -3856,1179 +3729,63 @@
     </row>
     <row r="47" spans="1:20">
       <c r="A47" t="s">
+        <v>161</v>
+      </c>
+      <c r="B47" t="s">
         <v>162</v>
       </c>
-      <c r="B47" t="s">
+      <c r="C47" t="s">
+        <v>159</v>
+      </c>
+      <c r="D47" t="s">
+        <v>59</v>
+      </c>
+      <c r="E47" t="s">
+        <v>100</v>
+      </c>
+      <c r="F47" s="1">
+        <v>5</v>
+      </c>
+      <c r="G47" s="1">
+        <v>6600</v>
+      </c>
+      <c r="H47" s="1">
+        <v>6600</v>
+      </c>
+      <c r="I47" s="1">
+        <v>6600</v>
+      </c>
+      <c r="J47" s="2">
+        <v>204930</v>
+      </c>
+      <c r="K47" s="3">
+        <v>0</v>
+      </c>
+      <c r="L47" s="3">
+        <v>7</v>
+      </c>
+      <c r="M47" s="4">
+        <v>677.41</v>
+      </c>
+      <c r="N47" s="4">
+        <v>0</v>
+      </c>
+      <c r="O47" t="s">
+        <v>25</v>
+      </c>
+      <c r="P47" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q47" s="3">
+        <v>18</v>
+      </c>
+      <c r="R47" t="s">
         <v>163</v>
       </c>
-      <c r="C47" t="s">
-        <v>154</v>
-      </c>
-      <c r="D47" t="s">
-        <v>22</v>
-      </c>
-      <c r="E47" t="s">
-        <v>67</v>
-      </c>
-      <c r="F47" s="1">
-        <v>1</v>
-      </c>
-      <c r="G47" s="1">
-        <v>23300</v>
-      </c>
-      <c r="H47" s="1">
-        <v>23300</v>
-      </c>
-      <c r="I47" s="1">
-        <v>23300</v>
-      </c>
-      <c r="J47" s="2">
-        <v>204574</v>
-      </c>
-      <c r="K47" s="3">
-        <v>0</v>
-      </c>
-      <c r="L47" s="3">
-        <v>9</v>
-      </c>
-      <c r="M47" s="2">
-        <v>613.72</v>
-      </c>
-      <c r="N47" s="2">
-        <v>0</v>
-      </c>
-      <c r="O47" t="s">
-        <v>25</v>
-      </c>
-      <c r="P47" s="1">
-        <v>0</v>
-      </c>
-      <c r="Q47" s="3">
-        <v>18</v>
-      </c>
-      <c r="R47" t="s">
-        <v>164</v>
-      </c>
       <c r="S47" t="s">
         <v>27</v>
       </c>
       <c r="T47" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="48" spans="1:20">
-      <c r="A48" t="s">
-        <v>165</v>
-      </c>
-      <c r="B48" t="s">
-        <v>166</v>
-      </c>
-      <c r="C48" t="s">
-        <v>154</v>
-      </c>
-      <c r="D48" t="s">
-        <v>22</v>
-      </c>
-      <c r="E48" t="s">
-        <v>67</v>
-      </c>
-      <c r="F48" s="1">
-        <v>1</v>
-      </c>
-      <c r="G48" s="1">
-        <v>10000</v>
-      </c>
-      <c r="H48" s="1">
-        <v>10000</v>
-      </c>
-      <c r="I48" s="1">
-        <v>10000</v>
-      </c>
-      <c r="J48" s="2">
-        <v>121800</v>
-      </c>
-      <c r="K48" s="3">
-        <v>0</v>
-      </c>
-      <c r="L48" s="3">
-        <v>7</v>
-      </c>
-      <c r="M48" s="2">
-        <v>284.2</v>
-      </c>
-      <c r="N48" s="2">
-        <v>0</v>
-      </c>
-      <c r="O48" t="s">
-        <v>25</v>
-      </c>
-      <c r="P48" s="1">
-        <v>0</v>
-      </c>
-      <c r="Q48" s="3">
-        <v>18</v>
-      </c>
-      <c r="R48" t="s">
-        <v>167</v>
-      </c>
-      <c r="S48" t="s">
-        <v>27</v>
-      </c>
-      <c r="T48" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="49" spans="1:20">
-      <c r="A49" t="s">
-        <v>168</v>
-      </c>
-      <c r="B49" t="s">
-        <v>169</v>
-      </c>
-      <c r="C49" t="s">
-        <v>154</v>
-      </c>
-      <c r="D49" t="s">
-        <v>22</v>
-      </c>
-      <c r="E49" t="s">
-        <v>67</v>
-      </c>
-      <c r="F49" s="1">
-        <v>1</v>
-      </c>
-      <c r="G49" s="1">
-        <v>1400</v>
-      </c>
-      <c r="H49" s="1">
-        <v>1400</v>
-      </c>
-      <c r="I49" s="1">
-        <v>1400</v>
-      </c>
-      <c r="J49" s="2">
-        <v>102312</v>
-      </c>
-      <c r="K49" s="3">
-        <v>0</v>
-      </c>
-      <c r="L49" s="3">
-        <v>5</v>
-      </c>
-      <c r="M49" s="2">
-        <v>170.52</v>
-      </c>
-      <c r="N49" s="2">
-        <v>0</v>
-      </c>
-      <c r="O49" t="s">
-        <v>25</v>
-      </c>
-      <c r="P49" s="1">
-        <v>0</v>
-      </c>
-      <c r="Q49" s="3">
-        <v>18</v>
-      </c>
-      <c r="R49" t="s">
-        <v>170</v>
-      </c>
-      <c r="S49" t="s">
-        <v>27</v>
-      </c>
-      <c r="T49" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="50" spans="1:20">
-      <c r="A50" t="s">
-        <v>171</v>
-      </c>
-      <c r="B50" t="s">
-        <v>172</v>
-      </c>
-      <c r="C50" t="s">
-        <v>154</v>
-      </c>
-      <c r="D50" t="s">
-        <v>22</v>
-      </c>
-      <c r="E50" t="s">
-        <v>67</v>
-      </c>
-      <c r="F50" s="1">
-        <v>1</v>
-      </c>
-      <c r="G50" s="1">
-        <v>3900</v>
-      </c>
-      <c r="H50" s="1">
-        <v>3900</v>
-      </c>
-      <c r="I50" s="1">
-        <v>3900</v>
-      </c>
-      <c r="J50" s="2">
-        <v>201630</v>
-      </c>
-      <c r="K50" s="3">
-        <v>0</v>
-      </c>
-      <c r="L50" s="3">
-        <v>7</v>
-      </c>
-      <c r="M50" s="2">
-        <v>470.47</v>
-      </c>
-      <c r="N50" s="2">
-        <v>0</v>
-      </c>
-      <c r="O50" t="s">
-        <v>25</v>
-      </c>
-      <c r="P50" s="1">
-        <v>0</v>
-      </c>
-      <c r="Q50" s="3">
-        <v>18</v>
-      </c>
-      <c r="R50" t="s">
-        <v>173</v>
-      </c>
-      <c r="S50" t="s">
-        <v>27</v>
-      </c>
-      <c r="T50" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="51" spans="1:20">
-      <c r="A51" t="s">
-        <v>174</v>
-      </c>
-      <c r="B51" t="s">
-        <v>175</v>
-      </c>
-      <c r="C51" t="s">
-        <v>176</v>
-      </c>
-      <c r="D51" t="s">
-        <v>22</v>
-      </c>
-      <c r="E51" t="s">
-        <v>67</v>
-      </c>
-      <c r="F51" s="1">
-        <v>1</v>
-      </c>
-      <c r="G51" s="1">
-        <v>7900</v>
-      </c>
-      <c r="H51" s="1">
-        <v>7900</v>
-      </c>
-      <c r="I51" s="1">
-        <v>7900</v>
-      </c>
-      <c r="J51" s="2">
-        <v>99382</v>
-      </c>
-      <c r="K51" s="3">
-        <v>0</v>
-      </c>
-      <c r="L51" s="3">
-        <v>8.5</v>
-      </c>
-      <c r="M51" s="2">
-        <v>305.05</v>
-      </c>
-      <c r="N51" s="2">
-        <v>0</v>
-      </c>
-      <c r="O51" t="s">
-        <v>25</v>
-      </c>
-      <c r="P51" s="1">
-        <v>0</v>
-      </c>
-      <c r="Q51" s="3">
-        <v>18</v>
-      </c>
-      <c r="R51" t="s">
-        <v>177</v>
-      </c>
-      <c r="S51" t="s">
-        <v>27</v>
-      </c>
-      <c r="T51" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="52" spans="1:20">
-      <c r="A52" t="s">
-        <v>152</v>
-      </c>
-      <c r="B52" t="s">
-        <v>153</v>
-      </c>
-      <c r="C52" t="s">
-        <v>176</v>
-      </c>
-      <c r="D52" t="s">
-        <v>22</v>
-      </c>
-      <c r="E52" t="s">
-        <v>67</v>
-      </c>
-      <c r="F52" s="1">
-        <v>1</v>
-      </c>
-      <c r="G52" s="1">
-        <v>3400</v>
-      </c>
-      <c r="H52" s="1">
-        <v>3400</v>
-      </c>
-      <c r="I52" s="1">
-        <v>3400</v>
-      </c>
-      <c r="J52" s="2">
-        <v>102272</v>
-      </c>
-      <c r="K52" s="3">
-        <v>0</v>
-      </c>
-      <c r="L52" s="3">
-        <v>8.5</v>
-      </c>
-      <c r="M52" s="2">
-        <v>313.92</v>
-      </c>
-      <c r="N52" s="2">
-        <v>0</v>
-      </c>
-      <c r="O52" t="s">
-        <v>25</v>
-      </c>
-      <c r="P52" s="1">
-        <v>0</v>
-      </c>
-      <c r="Q52" s="3">
-        <v>18</v>
-      </c>
-      <c r="R52" t="s">
-        <v>178</v>
-      </c>
-      <c r="S52" t="s">
-        <v>27</v>
-      </c>
-      <c r="T52" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="53" spans="1:20">
-      <c r="A53" t="s">
-        <v>83</v>
-      </c>
-      <c r="B53" t="s">
-        <v>84</v>
-      </c>
-      <c r="C53" t="s">
-        <v>176</v>
-      </c>
-      <c r="D53" t="s">
-        <v>42</v>
-      </c>
-      <c r="E53" t="s">
-        <v>179</v>
-      </c>
-      <c r="F53" s="1">
-        <v>14</v>
-      </c>
-      <c r="G53" s="1">
-        <v>19200</v>
-      </c>
-      <c r="H53" s="1">
-        <v>19200</v>
-      </c>
-      <c r="I53" s="1">
-        <v>19200</v>
-      </c>
-      <c r="J53" s="2">
-        <v>131904</v>
-      </c>
-      <c r="K53" s="3">
-        <v>0</v>
-      </c>
-      <c r="L53" s="3">
-        <v>9</v>
-      </c>
-      <c r="M53" s="2">
-        <v>428.69</v>
-      </c>
-      <c r="N53" s="2">
-        <v>0</v>
-      </c>
-      <c r="O53" t="s">
-        <v>25</v>
-      </c>
-      <c r="P53" s="1">
-        <v>0</v>
-      </c>
-      <c r="Q53" s="3">
-        <v>18</v>
-      </c>
-      <c r="R53" t="s">
-        <v>180</v>
-      </c>
-      <c r="S53" t="s">
-        <v>27</v>
-      </c>
-      <c r="T53" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="54" spans="1:20">
-      <c r="A54" t="s">
-        <v>134</v>
-      </c>
-      <c r="B54" t="s">
-        <v>135</v>
-      </c>
-      <c r="C54" t="s">
-        <v>176</v>
-      </c>
-      <c r="D54" t="s">
-        <v>31</v>
-      </c>
-      <c r="E54" t="s">
-        <v>22</v>
-      </c>
-      <c r="F54" s="1">
-        <v>0</v>
-      </c>
-      <c r="G54" s="1">
-        <v>100</v>
-      </c>
-      <c r="H54" s="1">
-        <v>100</v>
-      </c>
-      <c r="I54" s="1">
-        <v>0</v>
-      </c>
-      <c r="J54" s="2">
-        <v>12698</v>
-      </c>
-      <c r="K54" s="3">
-        <v>0</v>
-      </c>
-      <c r="L54" s="3">
-        <v>9</v>
-      </c>
-      <c r="M54" s="2">
-        <v>41.27</v>
-      </c>
-      <c r="N54" s="2">
-        <v>0</v>
-      </c>
-      <c r="O54" t="s">
-        <v>25</v>
-      </c>
-      <c r="P54" s="1">
-        <v>0</v>
-      </c>
-      <c r="Q54" s="3">
-        <v>18</v>
-      </c>
-      <c r="R54" t="s">
-        <v>181</v>
-      </c>
-      <c r="S54" t="s">
-        <v>27</v>
-      </c>
-      <c r="T54" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="55" spans="1:20">
-      <c r="A55" t="s">
-        <v>20</v>
-      </c>
-      <c r="B55" t="s">
-        <v>21</v>
-      </c>
-      <c r="C55" t="s">
-        <v>176</v>
-      </c>
-      <c r="D55" t="s">
-        <v>31</v>
-      </c>
-      <c r="E55" t="s">
-        <v>22</v>
-      </c>
-      <c r="F55" s="1">
-        <v>0</v>
-      </c>
-      <c r="G55" s="1">
-        <v>1500</v>
-      </c>
-      <c r="H55" s="1">
-        <v>1500</v>
-      </c>
-      <c r="I55" s="1">
-        <v>0</v>
-      </c>
-      <c r="J55" s="2">
-        <v>21060</v>
-      </c>
-      <c r="K55" s="3">
-        <v>0</v>
-      </c>
-      <c r="L55" s="3">
-        <v>5</v>
-      </c>
-      <c r="M55" s="2">
-        <v>38.02</v>
-      </c>
-      <c r="N55" s="2">
-        <v>0</v>
-      </c>
-      <c r="O55" t="s">
-        <v>25</v>
-      </c>
-      <c r="P55" s="1">
-        <v>0</v>
-      </c>
-      <c r="Q55" s="3">
-        <v>18</v>
-      </c>
-      <c r="R55" t="s">
-        <v>182</v>
-      </c>
-      <c r="S55" t="s">
-        <v>27</v>
-      </c>
-      <c r="T55" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="56" spans="1:20">
-      <c r="A56" t="s">
-        <v>183</v>
-      </c>
-      <c r="B56" t="s">
-        <v>184</v>
-      </c>
-      <c r="C56" t="s">
-        <v>176</v>
-      </c>
-      <c r="D56" t="s">
-        <v>42</v>
-      </c>
-      <c r="E56" t="s">
-        <v>179</v>
-      </c>
-      <c r="F56" s="1">
-        <v>14</v>
-      </c>
-      <c r="G56" s="1">
-        <v>4200</v>
-      </c>
-      <c r="H56" s="1">
-        <v>4200</v>
-      </c>
-      <c r="I56" s="1">
-        <v>4200</v>
-      </c>
-      <c r="J56" s="2">
-        <v>108360</v>
-      </c>
-      <c r="K56" s="3">
-        <v>0</v>
-      </c>
-      <c r="L56" s="3">
-        <v>7</v>
-      </c>
-      <c r="M56" s="2">
-        <v>273.91</v>
-      </c>
-      <c r="N56" s="2">
-        <v>0</v>
-      </c>
-      <c r="O56" t="s">
-        <v>25</v>
-      </c>
-      <c r="P56" s="1">
-        <v>0</v>
-      </c>
-      <c r="Q56" s="3">
-        <v>18</v>
-      </c>
-      <c r="R56" t="s">
-        <v>185</v>
-      </c>
-      <c r="S56" t="s">
-        <v>27</v>
-      </c>
-      <c r="T56" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="57" spans="1:20">
-      <c r="A57" t="s">
-        <v>186</v>
-      </c>
-      <c r="B57" t="s">
-        <v>187</v>
-      </c>
-      <c r="C57" t="s">
-        <v>176</v>
-      </c>
-      <c r="D57" t="s">
-        <v>31</v>
-      </c>
-      <c r="E57" t="s">
-        <v>22</v>
-      </c>
-      <c r="F57" s="1">
-        <v>0</v>
-      </c>
-      <c r="G57" s="1">
-        <v>1200</v>
-      </c>
-      <c r="H57" s="1">
-        <v>1200</v>
-      </c>
-      <c r="I57" s="1">
-        <v>0</v>
-      </c>
-      <c r="J57" s="2">
-        <v>110640</v>
-      </c>
-      <c r="K57" s="3">
-        <v>0</v>
-      </c>
-      <c r="L57" s="3">
-        <v>7</v>
-      </c>
-      <c r="M57" s="2">
-        <v>279.67</v>
-      </c>
-      <c r="N57" s="2">
-        <v>0</v>
-      </c>
-      <c r="O57" t="s">
-        <v>25</v>
-      </c>
-      <c r="P57" s="1">
-        <v>0</v>
-      </c>
-      <c r="Q57" s="3">
-        <v>18</v>
-      </c>
-      <c r="R57" t="s">
-        <v>188</v>
-      </c>
-      <c r="S57" t="s">
-        <v>27</v>
-      </c>
-      <c r="T57" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="58" spans="1:20">
-      <c r="A58" t="s">
-        <v>186</v>
-      </c>
-      <c r="B58" t="s">
-        <v>187</v>
-      </c>
-      <c r="C58" t="s">
-        <v>189</v>
-      </c>
-      <c r="D58" t="s">
-        <v>31</v>
-      </c>
-      <c r="E58" t="s">
-        <v>22</v>
-      </c>
-      <c r="F58" s="1">
-        <v>0</v>
-      </c>
-      <c r="G58" s="1">
-        <v>1200</v>
-      </c>
-      <c r="H58" s="1">
-        <v>1200</v>
-      </c>
-      <c r="I58" s="1">
-        <v>0</v>
-      </c>
-      <c r="J58" s="2">
-        <v>100680</v>
-      </c>
-      <c r="K58" s="3">
-        <v>0</v>
-      </c>
-      <c r="L58" s="3">
-        <v>8.5</v>
-      </c>
-      <c r="M58" s="2">
-        <v>332.8</v>
-      </c>
-      <c r="N58" s="2">
-        <v>0</v>
-      </c>
-      <c r="O58" t="s">
-        <v>25</v>
-      </c>
-      <c r="P58" s="1">
-        <v>0</v>
-      </c>
-      <c r="Q58" s="3">
-        <v>18</v>
-      </c>
-      <c r="R58" t="s">
-        <v>190</v>
-      </c>
-      <c r="S58" t="s">
-        <v>27</v>
-      </c>
-      <c r="T58" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="59" spans="1:20">
-      <c r="A59" t="s">
-        <v>191</v>
-      </c>
-      <c r="B59" t="s">
-        <v>192</v>
-      </c>
-      <c r="C59" t="s">
-        <v>189</v>
-      </c>
-      <c r="D59" t="s">
-        <v>31</v>
-      </c>
-      <c r="E59" t="s">
-        <v>22</v>
-      </c>
-      <c r="F59" s="1">
-        <v>0</v>
-      </c>
-      <c r="G59" s="1">
-        <v>6200</v>
-      </c>
-      <c r="H59" s="1">
-        <v>6200</v>
-      </c>
-      <c r="I59" s="1">
-        <v>0</v>
-      </c>
-      <c r="J59" s="2">
-        <v>95294</v>
-      </c>
-      <c r="K59" s="3">
-        <v>0</v>
-      </c>
-      <c r="L59" s="3">
-        <v>8.5</v>
-      </c>
-      <c r="M59" s="2">
-        <v>315</v>
-      </c>
-      <c r="N59" s="2">
-        <v>0</v>
-      </c>
-      <c r="O59" t="s">
-        <v>25</v>
-      </c>
-      <c r="P59" s="1">
-        <v>0</v>
-      </c>
-      <c r="Q59" s="3">
-        <v>18</v>
-      </c>
-      <c r="R59" t="s">
-        <v>193</v>
-      </c>
-      <c r="S59" t="s">
-        <v>27</v>
-      </c>
-      <c r="T59" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="60" spans="1:20">
-      <c r="A60" t="s">
-        <v>183</v>
-      </c>
-      <c r="B60" t="s">
-        <v>184</v>
-      </c>
-      <c r="C60" t="s">
-        <v>189</v>
-      </c>
-      <c r="D60" t="s">
-        <v>31</v>
-      </c>
-      <c r="E60" t="s">
-        <v>22</v>
-      </c>
-      <c r="F60" s="1">
-        <v>0</v>
-      </c>
-      <c r="G60" s="1">
-        <v>3700</v>
-      </c>
-      <c r="H60" s="1">
-        <v>3700</v>
-      </c>
-      <c r="I60" s="1">
-        <v>0</v>
-      </c>
-      <c r="J60" s="2">
-        <v>94720</v>
-      </c>
-      <c r="K60" s="3">
-        <v>0</v>
-      </c>
-      <c r="L60" s="3">
-        <v>8.5</v>
-      </c>
-      <c r="M60" s="2">
-        <v>313.1</v>
-      </c>
-      <c r="N60" s="2">
-        <v>0</v>
-      </c>
-      <c r="O60" t="s">
-        <v>25</v>
-      </c>
-      <c r="P60" s="1">
-        <v>0</v>
-      </c>
-      <c r="Q60" s="3">
-        <v>18</v>
-      </c>
-      <c r="R60" t="s">
-        <v>194</v>
-      </c>
-      <c r="S60" t="s">
-        <v>27</v>
-      </c>
-      <c r="T60" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="61" spans="1:20">
-      <c r="A61" t="s">
-        <v>195</v>
-      </c>
-      <c r="B61" t="s">
-        <v>196</v>
-      </c>
-      <c r="C61" t="s">
-        <v>189</v>
-      </c>
-      <c r="D61" t="s">
-        <v>31</v>
-      </c>
-      <c r="E61" t="s">
-        <v>22</v>
-      </c>
-      <c r="F61" s="1">
-        <v>0</v>
-      </c>
-      <c r="G61" s="1">
-        <v>4100</v>
-      </c>
-      <c r="H61" s="1">
-        <v>4100</v>
-      </c>
-      <c r="I61" s="1">
-        <v>0</v>
-      </c>
-      <c r="J61" s="2">
-        <v>98974</v>
-      </c>
-      <c r="K61" s="3">
-        <v>0</v>
-      </c>
-      <c r="L61" s="3">
-        <v>8.5</v>
-      </c>
-      <c r="M61" s="2">
-        <v>327.16</v>
-      </c>
-      <c r="N61" s="2">
-        <v>0</v>
-      </c>
-      <c r="O61" t="s">
-        <v>25</v>
-      </c>
-      <c r="P61" s="1">
-        <v>0</v>
-      </c>
-      <c r="Q61" s="3">
-        <v>18</v>
-      </c>
-      <c r="R61" t="s">
-        <v>197</v>
-      </c>
-      <c r="S61" t="s">
-        <v>27</v>
-      </c>
-      <c r="T61" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="62" spans="1:20">
-      <c r="A62" t="s">
-        <v>168</v>
-      </c>
-      <c r="B62" t="s">
-        <v>169</v>
-      </c>
-      <c r="C62" t="s">
-        <v>189</v>
-      </c>
-      <c r="D62" t="s">
-        <v>31</v>
-      </c>
-      <c r="E62" t="s">
-        <v>22</v>
-      </c>
-      <c r="F62" s="1">
-        <v>0</v>
-      </c>
-      <c r="G62" s="1">
-        <v>1500</v>
-      </c>
-      <c r="H62" s="1">
-        <v>1500</v>
-      </c>
-      <c r="I62" s="1">
-        <v>0</v>
-      </c>
-      <c r="J62" s="2">
-        <v>100200</v>
-      </c>
-      <c r="K62" s="3">
-        <v>0</v>
-      </c>
-      <c r="L62" s="3">
-        <v>8.5</v>
-      </c>
-      <c r="M62" s="2">
-        <v>331.22</v>
-      </c>
-      <c r="N62" s="2">
-        <v>0</v>
-      </c>
-      <c r="O62" t="s">
-        <v>25</v>
-      </c>
-      <c r="P62" s="1">
-        <v>0</v>
-      </c>
-      <c r="Q62" s="3">
-        <v>18</v>
-      </c>
-      <c r="R62" t="s">
-        <v>198</v>
-      </c>
-      <c r="S62" t="s">
-        <v>27</v>
-      </c>
-      <c r="T62" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="63" spans="1:20">
-      <c r="A63" t="s">
-        <v>86</v>
-      </c>
-      <c r="B63" t="s">
-        <v>87</v>
-      </c>
-      <c r="C63" t="s">
-        <v>199</v>
-      </c>
-      <c r="D63" t="s">
-        <v>42</v>
-      </c>
-      <c r="E63" t="s">
-        <v>100</v>
-      </c>
-      <c r="F63" s="1">
-        <v>10</v>
-      </c>
-      <c r="G63" s="1">
-        <v>1000</v>
-      </c>
-      <c r="H63" s="1">
-        <v>1000</v>
-      </c>
-      <c r="I63" s="1">
-        <v>1000</v>
-      </c>
-      <c r="J63" s="2">
-        <v>83100</v>
-      </c>
-      <c r="K63" s="3">
-        <v>0</v>
-      </c>
-      <c r="L63" s="3">
-        <v>9</v>
-      </c>
-      <c r="M63" s="2">
-        <v>311.63</v>
-      </c>
-      <c r="N63" s="2">
-        <v>0</v>
-      </c>
-      <c r="O63" t="s">
-        <v>25</v>
-      </c>
-      <c r="P63" s="1">
-        <v>0</v>
-      </c>
-      <c r="Q63" s="3">
-        <v>18</v>
-      </c>
-      <c r="R63" t="s">
-        <v>200</v>
-      </c>
-      <c r="S63" t="s">
-        <v>27</v>
-      </c>
-      <c r="T63" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="64" spans="1:20">
-      <c r="A64" t="s">
-        <v>201</v>
-      </c>
-      <c r="B64" t="s">
-        <v>202</v>
-      </c>
-      <c r="C64" t="s">
-        <v>199</v>
-      </c>
-      <c r="D64" t="s">
-        <v>59</v>
-      </c>
-      <c r="E64" t="s">
-        <v>103</v>
-      </c>
-      <c r="F64" s="1">
-        <v>7</v>
-      </c>
-      <c r="G64" s="1">
-        <v>6600</v>
-      </c>
-      <c r="H64" s="1">
-        <v>6600</v>
-      </c>
-      <c r="I64" s="1">
-        <v>6600</v>
-      </c>
-      <c r="J64" s="2">
-        <v>204930</v>
-      </c>
-      <c r="K64" s="3">
-        <v>0</v>
-      </c>
-      <c r="L64" s="3">
-        <v>7</v>
-      </c>
-      <c r="M64" s="2">
-        <v>597.71</v>
-      </c>
-      <c r="N64" s="2">
-        <v>0</v>
-      </c>
-      <c r="O64" t="s">
-        <v>25</v>
-      </c>
-      <c r="P64" s="1">
-        <v>0</v>
-      </c>
-      <c r="Q64" s="3">
-        <v>18</v>
-      </c>
-      <c r="R64" t="s">
-        <v>203</v>
-      </c>
-      <c r="S64" t="s">
-        <v>27</v>
-      </c>
-      <c r="T64" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="65" spans="1:20">
-      <c r="A65" t="s">
-        <v>204</v>
-      </c>
-      <c r="B65" t="s">
-        <v>205</v>
-      </c>
-      <c r="C65" t="s">
-        <v>199</v>
-      </c>
-      <c r="D65" t="s">
-        <v>31</v>
-      </c>
-      <c r="E65" t="s">
-        <v>22</v>
-      </c>
-      <c r="F65" s="1">
-        <v>0</v>
-      </c>
-      <c r="G65" s="1">
-        <v>3800</v>
-      </c>
-      <c r="H65" s="1">
-        <v>3800</v>
-      </c>
-      <c r="I65" s="1">
-        <v>0</v>
-      </c>
-      <c r="J65" s="2">
-        <v>224466</v>
-      </c>
-      <c r="K65" s="3">
-        <v>0</v>
-      </c>
-      <c r="L65" s="3">
-        <v>7</v>
-      </c>
-      <c r="M65" s="2">
-        <v>654.69</v>
-      </c>
-      <c r="N65" s="2">
-        <v>0</v>
-      </c>
-      <c r="O65" t="s">
-        <v>25</v>
-      </c>
-      <c r="P65" s="1">
-        <v>0</v>
-      </c>
-      <c r="Q65" s="3">
-        <v>18</v>
-      </c>
-      <c r="R65" t="s">
-        <v>206</v>
-      </c>
-      <c r="S65" t="s">
-        <v>27</v>
-      </c>
-      <c r="T65" t="s">
         <v>28</v>
       </c>
     </row>

</xml_diff>